<commit_message>
Add textures to car
</commit_message>
<xml_diff>
--- a/tpTP/text.xlsx
+++ b/tpTP/text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Silva\Desktop\cgra\tpTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30623D83-C627-4FF2-BA36-01DDBCCEA5C2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D4033-DFAF-4B77-858A-4A2B310EB851}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8970" windowHeight="6390" xr2:uid="{63EEBBA1-5ADA-44A6-9475-D72E2D3BC3D0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,8 +34,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,54 +51,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -99,40 +70,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color indexed="64"/>
-      </diagonal>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color indexed="64"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,15 +102,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>13138</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
+      <xdr:rowOff>42892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1042147</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>11207</xdr:rowOff>
+      <xdr:colOff>1055285</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2382603</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -178,14 +125,20 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2117912" y="56030"/>
-          <a:ext cx="1042147" cy="2342030"/>
+          <a:off x="2128345" y="42892"/>
+          <a:ext cx="1042147" cy="2339711"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
             <a:gd name="adj" fmla="val 100000"/>
           </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -217,15 +170,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6724</xdr:colOff>
+      <xdr:colOff>155</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>29137</xdr:rowOff>
+      <xdr:rowOff>42275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1048871</xdr:colOff>
+      <xdr:colOff>1042302</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2371167</xdr:rowOff>
+      <xdr:rowOff>2384305</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -240,7 +193,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6349253" y="29137"/>
+          <a:off x="6345776" y="42275"/>
           <a:ext cx="1042147" cy="2342030"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -248,6 +201,12 @@
             <a:gd name="adj" fmla="val 0"/>
           </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -310,6 +269,12 @@
             <a:gd name="adj" fmla="val 0"/>
           </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -340,14 +305,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3155575</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2470</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>2382369</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>22411</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1051033</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>22410</xdr:rowOff>
     </xdr:to>
@@ -364,14 +329,20 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6326840" y="4769222"/>
-          <a:ext cx="1091453" cy="2413747"/>
+          <a:off x="6348091" y="4766903"/>
+          <a:ext cx="1048563" cy="2409110"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
             <a:gd name="adj" fmla="val 100000"/>
           </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -398,6 +369,197 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1057602</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>717176</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1524000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8185886-8723-40E5-81B4-778D16062699}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3172809" y="717176"/>
+          <a:ext cx="3179381" cy="806824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1037664</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>712693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3172810</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1519517</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41B614B1-E5AC-43CF-AB1A-7C0D4D207B65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3152871" y="5481762"/>
+          <a:ext cx="3192749" cy="806824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1043874</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>265923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2140325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2231004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Image result for ambulance sign">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2820780A-A3EF-4A82-A041-F02D6CA6F153}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="52003"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4215139" y="7426482"/>
+          <a:ext cx="1096451" cy="1965081"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -700,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8170AAD1-9532-456E-ADC7-F8E30933A8F9}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,25 +877,42 @@
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="10"/>
+    <row r="1" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6"/>
+    <row r="2" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="9"/>
+    <row r="3" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="8"/>
+    <row r="4" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>